<commit_message>
widen the length of the columns
</commit_message>
<xml_diff>
--- a/find_spreadsheet_here/test-folder.xlsx
+++ b/find_spreadsheet_here/test-folder.xlsx
@@ -407,6 +407,20 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
change 'difficulty' to 'understanding'
</commit_message>
<xml_diff>
--- a/find_spreadsheet_here/test-folder.xlsx
+++ b/find_spreadsheet_here/test-folder.xlsx
@@ -22,7 +22,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Difficulty</t>
+    <t>Understanding</t>
   </si>
   <si>
     <t>content-1</t>
@@ -85,12 +85,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,7 +113,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,27 +408,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,171 +428,237 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="G11" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="J11" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>